<commit_message>
Reemplazo de contenido con versión actualizada
</commit_message>
<xml_diff>
--- a/Otros_parámetros.xlsx
+++ b/Otros_parámetros.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://latamlogistics.sharepoint.com/sites/LatamLogistics/Documentos compartidos/P24-P018-Opain Simulation Tool/05. Documentación/02 APP/V20_Versión prueba a publicar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://latamlogistics.sharepoint.com/sites/LatamLogistics/Documentos compartidos/P24-P018-Opain Simulation Tool/05. Documentación/02 APP/V22_Versión planes futuros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{28220AFD-3AB5-4D08-8B56-549991F11602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{154957A8-2E79-4D24-980E-00C93FE970FA}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{28220AFD-3AB5-4D08-8B56-549991F11602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27265B83-EE34-499D-B21C-68A0FFCF44A5}"/>
   <bookViews>
-    <workbookView xWindow="35970" yWindow="0" windowWidth="21630" windowHeight="11250" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lines Capacity" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="102">
   <si>
     <t>MU08_2</t>
   </si>
@@ -241,97 +241,100 @@
     <t>Others</t>
   </si>
   <si>
-    <t>LA</t>
-  </si>
-  <si>
-    <t>AV</t>
-  </si>
-  <si>
-    <t>DL</t>
-  </si>
-  <si>
-    <t>NK</t>
-  </si>
-  <si>
-    <t>B6</t>
-  </si>
-  <si>
-    <t>IB</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>Y4</t>
-  </si>
-  <si>
-    <t>9R</t>
-  </si>
-  <si>
-    <t>CM</t>
-  </si>
-  <si>
-    <t>UA</t>
-  </si>
-  <si>
-    <t>AM</t>
-  </si>
-  <si>
-    <t>9V</t>
-  </si>
-  <si>
-    <t>UX</t>
-  </si>
-  <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>KL</t>
-  </si>
-  <si>
-    <t>EK</t>
-  </si>
-  <si>
-    <t>TK</t>
-  </si>
-  <si>
-    <t>DM</t>
-  </si>
-  <si>
-    <t>AR</t>
-  </si>
-  <si>
-    <t>AF</t>
-  </si>
-  <si>
-    <t>VB</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
-    <t>T9</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>PU</t>
-  </si>
-  <si>
-    <t>LH</t>
-  </si>
-  <si>
-    <t>QL</t>
-  </si>
-  <si>
-    <t>VE</t>
-  </si>
-  <si>
-    <t>JA</t>
+    <t>Avianca</t>
+  </si>
+  <si>
+    <t>Aerolineas</t>
+  </si>
+  <si>
+    <t>Aeromexico</t>
+  </si>
+  <si>
+    <t>Aircanada</t>
+  </si>
+  <si>
+    <t>Aireuropa</t>
+  </si>
+  <si>
+    <t>Airfrance</t>
+  </si>
+  <si>
+    <t>American</t>
+  </si>
+  <si>
+    <t>Clic</t>
+  </si>
+  <si>
+    <t>Copa</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Emirates</t>
+  </si>
+  <si>
+    <t>Gol</t>
+  </si>
+  <si>
+    <t>Iberia</t>
+  </si>
+  <si>
+    <t>Jetsmart</t>
+  </si>
+  <si>
+    <t>Klm</t>
+  </si>
+  <si>
+    <t>Laser</t>
+  </si>
+  <si>
+    <t>Latam</t>
+  </si>
+  <si>
+    <t>Lufthansa</t>
+  </si>
+  <si>
+    <t>Satena</t>
+  </si>
+  <si>
+    <t>Spirit</t>
+  </si>
+  <si>
+    <t>Taca</t>
+  </si>
+  <si>
+    <t>Turkish</t>
+  </si>
+  <si>
+    <t>United</t>
+  </si>
+  <si>
+    <t>Vivaaerobus</t>
+  </si>
+  <si>
+    <t>Wingo</t>
+  </si>
+  <si>
+    <t>Avior</t>
+  </si>
+  <si>
+    <t>Skyairline</t>
+  </si>
+  <si>
+    <t>Turpial</t>
+  </si>
+  <si>
+    <t>Volaris</t>
+  </si>
+  <si>
+    <t>Arajet</t>
+  </si>
+  <si>
+    <t>Jetblue</t>
+  </si>
+  <si>
+    <t>Plus</t>
   </si>
 </sst>
 </file>
@@ -1232,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982AAAA0-9337-416E-89F4-09BD40450ECF}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,7 +1256,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -1264,7 +1267,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -1275,7 +1278,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -1286,7 +1289,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -1297,7 +1300,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -1308,7 +1311,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -1316,7 +1319,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1324,7 +1327,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -1332,7 +1335,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -1340,7 +1343,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -1348,7 +1351,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
@@ -1356,7 +1359,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
@@ -1364,7 +1367,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
@@ -1372,7 +1375,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
@@ -1380,7 +1383,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
@@ -1388,7 +1391,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -1396,7 +1399,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -1404,7 +1407,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -1412,7 +1415,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -1420,7 +1423,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
@@ -1428,7 +1431,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
@@ -1436,7 +1439,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
@@ -1444,7 +1447,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
@@ -1452,7 +1455,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
@@ -1460,15 +1463,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
         <v>19</v>
@@ -1476,7 +1479,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
         <v>19</v>
@@ -1484,7 +1487,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
         <v>19</v>
@@ -1492,7 +1495,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
         <v>19</v>
@@ -1508,7 +1511,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
         <v>19</v>
@@ -1516,7 +1519,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B33" t="s">
         <v>19</v>
@@ -1524,17 +1527,25 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1548,7 +1559,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1563,27 +1574,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1593,10 +1604,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCA57BC-1267-4483-A194-FC498938287E}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1617,7 +1628,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1625,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1633,7 +1644,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1641,7 +1652,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -1652,7 +1663,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1660,7 +1671,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1668,7 +1679,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1676,7 +1687,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1684,7 +1695,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1692,7 +1703,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1700,7 +1711,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1708,7 +1719,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1716,7 +1727,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1724,7 +1735,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1732,7 +1743,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1748,7 +1759,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1756,7 +1767,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1764,7 +1775,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1772,7 +1783,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1780,7 +1791,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1788,15 +1799,15 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1804,7 +1815,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1812,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1820,7 +1831,7 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1828,7 +1839,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1836,15 +1847,15 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1852,18 +1863,15 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" t="s">
         <v>15</v>
@@ -1871,10 +1879,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
         <v>15</v>
@@ -1882,21 +1890,21 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C35" t="s">
         <v>14</v>
@@ -1904,10 +1912,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
@@ -1915,12 +1923,23 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
         <v>70</v>
       </c>
       <c r="C37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1933,8 +1952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8EBE50-D669-4040-B488-D5F0358CD3CF}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1955,7 +1974,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
@@ -1969,7 +1988,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -1983,7 +2002,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -1997,7 +2016,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -2043,15 +2062,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D51B4EF6D435BF4087A9F3D0F2DDD6E6" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a4d6df66db5087d4afd2ed0df6e4b748">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cb1ebd1e-73bd-4435-9ddb-e457d802b192" xmlns:ns3="1d610826-33ee-436b-98dd-31071ee94393" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01439f4cb1db2f104cac49d7e581fce5" ns2:_="" ns3:_="">
     <xsd:import namespace="cb1ebd1e-73bd-4435-9ddb-e457d802b192"/>
@@ -2286,15 +2296,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91F93E24-C41E-4025-9E34-B91217385A64}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D89FD2F7-3D61-4AB5-9601-D2B9130F2A4D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2311,4 +2322,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91F93E24-C41E-4025-9E34-B91217385A64}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>